<commit_message>
Fix handling of format, especially for dates. Time part of date format is not supported. Fix handling of shared strings when a string is split in multiple runs. First attempts at creating xml file required to write xlsx files.
</commit_message>
<xml_diff>
--- a/test_xlsx_data/test_file_1.xlsx
+++ b/test_xlsx_data/test_file_1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27948" windowHeight="12372"/>
+    <workbookView windowHeight="17680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Pick up Information</t>
     </r>
@@ -60,7 +60,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Company</t>
     </r>
@@ -80,13 +80,16 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>:</t>
     </r>
   </si>
   <si>
     <t>Date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3-2-2025</t>
   </si>
   <si>
     <r>
@@ -95,7 +98,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Address</t>
     </r>
@@ -115,13 +118,13 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>:</t>
     </r>
   </si>
   <si>
-    <t>Plateau de l'Aigle 7, 1474 Genappe, Belgium</t>
+    <t>Rue du Puit, 123 Bruxelles 1020 /Belgium</t>
   </si>
   <si>
     <t>Transport Clause:</t>
@@ -136,7 +139,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Contact</t>
     </r>
@@ -156,13 +159,13 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>:</t>
     </r>
   </si>
   <si>
-    <t>Li Ling</t>
+    <t>Dupont &amp;  Dupond</t>
   </si>
   <si>
     <r>
@@ -171,7 +174,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Phone</t>
     </r>
@@ -191,13 +194,13 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>:</t>
     </r>
   </si>
   <si>
-    <t>+32   0496754614</t>
+    <t>+32   012345678</t>
   </si>
   <si>
     <t>EORI No.:</t>
@@ -218,7 +221,7 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Delivery Information</t>
     </r>
@@ -234,7 +237,18 @@
     </r>
   </si>
   <si>
-    <t>Room 3019, 3rd Floor, Jinchi Center, No.1 Sanwei South Road, Xixiang, Baoan District, Shenzhen City, Guangdong 518126</t>
+    <r>
+      <t xml:space="preserve">Somewhere in China
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中国某地</t>
+    </r>
   </si>
   <si>
     <r>
@@ -243,7 +257,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Contact</t>
     </r>
@@ -263,23 +277,23 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>:</t>
     </r>
   </si>
   <si>
-    <t>Jiang Nan</t>
+    <t>Zhang Chongren</t>
   </si>
   <si>
     <t xml:space="preserve">
-0755-15252740</t>
+0086-123456789</t>
   </si>
   <si>
     <t>邮箱:</t>
   </si>
   <si>
-    <t>jiangchigo@gmail.com</t>
+    <t>chongren@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">MARKS &amp; NOS   </t>
@@ -291,7 +305,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Ctns</t>
     </r>
@@ -313,7 +327,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Description</t>
     </r>
@@ -335,7 +349,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Quanitity</t>
     </r>
@@ -357,7 +371,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">Unit Value     </t>
     </r>
@@ -379,7 +393,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">Total Value      </t>
     </r>
@@ -395,43 +409,16 @@
     </r>
   </si>
   <si>
-    <t>No. of Pallet/Ctn:  7Ctns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  3-2-2025</t>
-    <phoneticPr fontId="25" type="noConversion"/>
-  </si>
-  <si>
-    <t>75 world stamps collections 
-(in 74 albums,1 bag)</t>
-    <phoneticPr fontId="25" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 536.8 EUR(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>欧元</t>
-    </r>
+    <t>Something of value</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="25" type="noConversion"/>
-  </si>
-  <si>
-    <r>
+        <charset val="134"/>
+      </rPr>
       <t>7.16 EUR(</t>
     </r>
     <r>
@@ -448,14 +435,51 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>)</t>
     </r>
-    <phoneticPr fontId="25" type="noConversion"/>
-  </si>
-  <si>
-    <r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 536.8 EUR(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>欧元</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>No. of Pallet/Ctn:  7Ctns</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>重量(Weigh)：18kg,</t>
     </r>
     <r>
@@ -463,7 +487,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>20</t>
@@ -482,7 +505,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>7</t>
@@ -501,7 +523,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>15</t>
@@ -520,7 +541,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>19</t>
@@ -539,7 +559,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -558,7 +577,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>20</t>
@@ -572,10 +590,15 @@
       </rPr>
       <t>kg</t>
     </r>
-    <phoneticPr fontId="25" type="noConversion"/>
-  </si>
-  <si>
-    <r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>尺寸(Size)：</t>
     </r>
     <r>
@@ -583,7 +606,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>50</t>
@@ -602,7 +624,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -621,7 +642,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -640,7 +660,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -659,7 +678,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -678,7 +696,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -697,7 +714,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -716,7 +732,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>30</t>
@@ -735,7 +750,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -754,7 +768,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -773,7 +786,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -792,7 +804,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -811,7 +822,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>30</t>
@@ -830,7 +840,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>49</t>
@@ -849,7 +858,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>38</t>
@@ -868,7 +876,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -887,7 +894,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>39</t>
@@ -906,7 +912,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>8</t>
@@ -925,7 +930,6 @@
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>38</t>
@@ -939,18 +943,21 @@
       </rPr>
       <t>cm</t>
     </r>
-    <phoneticPr fontId="25" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="178" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;€&quot;#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="\$#,##0.00;[Red]\$#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;€&quot;#,##0.00\)"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -961,122 +968,273 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="22"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1086,6 +1244,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -1093,9 +1257,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
+      <sz val="12"/>
+      <name val="宋体-简"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1105,28 +1268,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1139,8 +1282,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1167,15 +1496,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1275,9 +1595,260 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1297,194 +1868,241 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="13" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="17" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1495,7 +2113,80 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>215900</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>698500</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>495300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5974715" y="1308735"/>
+              <a:ext cx="1465580" cy="495300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vert="horz" wrap="square" anchor="ctr" upright="1"/>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="SimSun" charset="-122"/>
+                  <a:ea typeface="SimSun" charset="-122"/>
+                  <a:cs typeface="SimSun" charset="-122"/>
+                  <a:sym typeface="SimSun" charset="-122"/>
+                </a:rPr>
+                <a:t>   Door to Door</a:t>
+              </a:r>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="SimSun" charset="-122"/>
+                <a:ea typeface="SimSun" charset="-122"/>
+                <a:cs typeface="SimSun" charset="-122"/>
+                <a:sym typeface="SimSun" charset="-122"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1821,311 +2512,342 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.1057692307692" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.4423076923077" style="4" customWidth="1"/>
+    <col min="3" max="3" width="31.1057692307692" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.6634615384615" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.8846153846154" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.8846153846154" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.8846153846154" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.05" customHeight="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" ht="43.05" customHeight="1" spans="1:6">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1">
-      <c r="A2" s="45" t="s">
+    <row r="2" ht="30" customHeight="1" spans="1:5">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="44"/>
     </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" ht="30" customHeight="1" spans="1:6">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" ht="52.05" customHeight="1" spans="1:6">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:6">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:6">
+      <c r="A8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="52"/>
+    </row>
+    <row r="9" ht="9" customHeight="1" spans="2:5">
+      <c r="B9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="54"/>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:6">
+      <c r="A10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="56"/>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:6">
+      <c r="A11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" ht="57" customHeight="1" spans="1:6">
+      <c r="A12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="54"/>
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="1:6">
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="54"/>
+    </row>
+    <row r="14" ht="30" customHeight="1" spans="1:6">
+      <c r="A14" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="54"/>
+    </row>
+    <row r="15" ht="30" customHeight="1" spans="1:6">
+      <c r="A15" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="54"/>
+    </row>
+    <row r="16" ht="12" customHeight="1"/>
+    <row r="17" s="2" customFormat="1" ht="39" customHeight="1" spans="1:6">
+      <c r="A17" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" ht="30" customHeight="1" spans="1:6">
+      <c r="A18" s="36"/>
+      <c r="B18" s="37">
+        <v>7</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>30</v>
       </c>
+      <c r="D18" s="37">
+        <v>75</v>
+      </c>
+      <c r="E18" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="52.05" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="19" ht="30" customHeight="1" spans="1:6">
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="10"/>
+    <row r="20" ht="30" customHeight="1" spans="1:6">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
+    <row r="21" ht="30" customHeight="1" spans="1:6">
+      <c r="A21" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
     </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
-      <c r="A7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+    <row r="22" ht="34.05" customHeight="1" spans="1:6">
+      <c r="A22" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
     </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
-      <c r="A8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="9" customHeight="1">
-      <c r="B9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
-      <c r="A10" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="57" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
-      <c r="A14" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1">
-      <c r="A15" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="12" customHeight="1"/>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="39" customHeight="1">
-      <c r="A17" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34">
-        <v>7</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="34">
-        <v>75</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1">
-      <c r="A21" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-    </row>
-    <row r="22" spans="1:6" ht="34.049999999999997" customHeight="1">
-      <c r="A22" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-    </row>
-    <row r="23" spans="1:6" ht="72" customHeight="1">
-      <c r="A23" s="65" t="s">
+    <row r="23" ht="72" customHeight="1" spans="1:6">
+      <c r="A23" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
   </sheetData>
   <sortState ref="B20:H58">
     <sortCondition ref="B20:B58"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A23:F23"/>
   </mergeCells>
-  <phoneticPr fontId="25" type="noConversion"/>
-  <pageMargins left="0.70833333333333304" right="0.35416666666666702" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31388888888888899" footer="0.31388888888888899"/>
-  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId4" display="chongren@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.708333333333333" right="0.354166666666667" top="0.747916666666667" bottom="0.747916666666667" header="0.313888888888889" footer="0.313888888888889"/>
+  <pageSetup paperSize="1" scale="80" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" name="Check Box 5" r:id="rId3">
+              <controlPr defaultSize="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>215900</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>698500</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>495300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>